<commit_message>
Hikari OCR app initial push to listman branch
</commit_message>
<xml_diff>
--- a/template_output.xlsx
+++ b/template_output.xlsx
@@ -1578,38 +1578,26 @@
           <t>一律</t>
         </is>
       </c>
-      <c r="B21" s="44" t="inlineStr">
-        <is>
-          <t>53462</t>
-        </is>
-      </c>
-      <c r="C21" s="50" t="inlineStr">
-        <is>
-          <t>58907</t>
-        </is>
-      </c>
-      <c r="D21" s="44" t="inlineStr">
-        <is>
-          <t>60872</t>
-        </is>
-      </c>
-      <c r="E21" s="44" t="inlineStr">
-        <is>
-          <t>29383</t>
-        </is>
-      </c>
-      <c r="F21" s="44" t="inlineStr">
-        <is>
-          <t>28637</t>
-        </is>
-      </c>
-      <c r="G21" s="44" t="n"/>
-      <c r="H21" s="44" t="n"/>
-      <c r="I21" s="44" t="n"/>
-      <c r="J21" s="44" t="n"/>
-      <c r="K21" s="44" t="n"/>
-      <c r="L21" s="44" t="n"/>
-      <c r="M21" s="44" t="n"/>
+      <c r="B21" s="44" t="inlineStr"/>
+      <c r="C21" s="50" t="inlineStr"/>
+      <c r="D21" s="44" t="inlineStr"/>
+      <c r="E21" s="44" t="inlineStr"/>
+      <c r="F21" s="44" t="inlineStr"/>
+      <c r="G21" s="44" t="inlineStr"/>
+      <c r="H21" s="44" t="inlineStr"/>
+      <c r="I21" s="44" t="inlineStr"/>
+      <c r="J21" s="44" t="inlineStr">
+        <is>
+          <t>13819</t>
+        </is>
+      </c>
+      <c r="K21" s="44" t="inlineStr">
+        <is>
+          <t>13812</t>
+        </is>
+      </c>
+      <c r="L21" s="44" t="inlineStr"/>
+      <c r="M21" s="44" t="inlineStr"/>
       <c r="N21" s="44" t="n"/>
     </row>
     <row r="22">

</xml_diff>

<commit_message>
OCR app initial push to main
</commit_message>
<xml_diff>
--- a/template_output.xlsx
+++ b/template_output.xlsx
@@ -1270,11 +1270,7 @@
           <t>法人名</t>
         </is>
       </c>
-      <c r="B1" s="71" t="inlineStr">
-        <is>
-          <t>渡辺株式会社</t>
-        </is>
-      </c>
+      <c r="B1" s="71" t="inlineStr"/>
       <c r="C1" s="86" t="n"/>
       <c r="D1" s="87" t="n"/>
     </row>
@@ -1578,24 +1574,36 @@
           <t>一律</t>
         </is>
       </c>
-      <c r="B21" s="44" t="inlineStr"/>
-      <c r="C21" s="50" t="inlineStr"/>
-      <c r="D21" s="44" t="inlineStr"/>
-      <c r="E21" s="44" t="inlineStr"/>
-      <c r="F21" s="44" t="inlineStr"/>
+      <c r="B21" s="44" t="inlineStr">
+        <is>
+          <t>53462</t>
+        </is>
+      </c>
+      <c r="C21" s="50" t="inlineStr">
+        <is>
+          <t>58907</t>
+        </is>
+      </c>
+      <c r="D21" s="44" t="inlineStr">
+        <is>
+          <t>60872</t>
+        </is>
+      </c>
+      <c r="E21" s="44" t="inlineStr">
+        <is>
+          <t>29383</t>
+        </is>
+      </c>
+      <c r="F21" s="44" t="inlineStr">
+        <is>
+          <t>28637</t>
+        </is>
+      </c>
       <c r="G21" s="44" t="inlineStr"/>
       <c r="H21" s="44" t="inlineStr"/>
       <c r="I21" s="44" t="inlineStr"/>
-      <c r="J21" s="44" t="inlineStr">
-        <is>
-          <t>13819</t>
-        </is>
-      </c>
-      <c r="K21" s="44" t="inlineStr">
-        <is>
-          <t>13812</t>
-        </is>
-      </c>
+      <c r="J21" s="44" t="inlineStr"/>
+      <c r="K21" s="44" t="inlineStr"/>
       <c r="L21" s="44" t="inlineStr"/>
       <c r="M21" s="44" t="inlineStr"/>
       <c r="N21" s="44" t="n"/>

</xml_diff>

<commit_message>
Add deployment configs and OCR quality features
</commit_message>
<xml_diff>
--- a/template_output.xlsx
+++ b/template_output.xlsx
@@ -1270,7 +1270,11 @@
           <t>法人名</t>
         </is>
       </c>
-      <c r="B1" s="71" t="inlineStr"/>
+      <c r="B1" s="71" t="inlineStr">
+        <is>
+          <t>あああ</t>
+        </is>
+      </c>
       <c r="C1" s="86" t="n"/>
       <c r="D1" s="87" t="n"/>
     </row>
@@ -1576,20 +1580,64 @@
       </c>
       <c r="B21" s="44" t="inlineStr">
         <is>
-          <t>223487</t>
-        </is>
-      </c>
-      <c r="C21" s="50" t="inlineStr"/>
-      <c r="D21" s="44" t="inlineStr"/>
-      <c r="E21" s="44" t="inlineStr"/>
-      <c r="F21" s="44" t="inlineStr"/>
-      <c r="G21" s="44" t="inlineStr"/>
-      <c r="H21" s="44" t="inlineStr"/>
-      <c r="I21" s="44" t="inlineStr"/>
-      <c r="J21" s="44" t="inlineStr"/>
-      <c r="K21" s="44" t="inlineStr"/>
-      <c r="L21" s="44" t="inlineStr"/>
-      <c r="M21" s="44" t="inlineStr"/>
+          <t>34100</t>
+        </is>
+      </c>
+      <c r="C21" s="50" t="inlineStr">
+        <is>
+          <t>43360</t>
+        </is>
+      </c>
+      <c r="D21" s="44" t="inlineStr">
+        <is>
+          <t>44524</t>
+        </is>
+      </c>
+      <c r="E21" s="44" t="inlineStr">
+        <is>
+          <t>52037</t>
+        </is>
+      </c>
+      <c r="F21" s="44" t="inlineStr">
+        <is>
+          <t>38711</t>
+        </is>
+      </c>
+      <c r="G21" s="44" t="inlineStr">
+        <is>
+          <t>44791</t>
+        </is>
+      </c>
+      <c r="H21" s="44" t="inlineStr">
+        <is>
+          <t>36589</t>
+        </is>
+      </c>
+      <c r="I21" s="44" t="inlineStr">
+        <is>
+          <t>35305</t>
+        </is>
+      </c>
+      <c r="J21" s="44" t="inlineStr">
+        <is>
+          <t>52966</t>
+        </is>
+      </c>
+      <c r="K21" s="44" t="inlineStr">
+        <is>
+          <t>38854</t>
+        </is>
+      </c>
+      <c r="L21" s="44" t="inlineStr">
+        <is>
+          <t>46427</t>
+        </is>
+      </c>
+      <c r="M21" s="44" t="inlineStr">
+        <is>
+          <t>44077</t>
+        </is>
+      </c>
       <c r="N21" s="44" t="n"/>
     </row>
     <row r="22">

</xml_diff>